<commit_message>
finish UI Training, responsive
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\xampp\htdocs\Calisthenics\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Calisthenics\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Thời gian</t>
   </si>
@@ -135,12 +135,15 @@
   </si>
   <si>
     <t>noel rồi</t>
+  </si>
+  <si>
+    <t>Tuần cuối dựng layout cho màn hình quản lý, làm chức năng quản lý các bài post</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -171,7 +174,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,6 +199,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -210,11 +219,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -223,6 +231,16 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -506,23 +524,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="56.42578125" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" style="9" customWidth="1"/>
+    <col min="3" max="3" width="65.42578125" customWidth="1"/>
+    <col min="4" max="4" width="84.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -536,7 +554,7 @@
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="8">
         <v>43436</v>
       </c>
       <c r="C2" t="s">
@@ -547,18 +565,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="3">
+      <c r="B3" s="8">
         <v>43437</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
+      <c r="B4" s="8">
         <v>43438</v>
       </c>
       <c r="C4" t="s">
@@ -568,19 +586,19 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="B5" s="3">
+    <row r="5" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
         <v>43439</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
+      <c r="B6" s="8">
         <v>43440</v>
       </c>
       <c r="C6" t="s">
@@ -588,7 +606,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="3">
+      <c r="B7" s="8">
         <v>43441</v>
       </c>
       <c r="C7" t="s">
@@ -599,7 +617,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="3">
+      <c r="B8" s="8">
         <v>43442</v>
       </c>
       <c r="C8" t="s">
@@ -610,7 +628,7 @@
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="8">
         <v>43444</v>
       </c>
       <c r="C10" t="s">
@@ -618,18 +636,18 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B11" s="3">
+      <c r="B11" s="8">
         <v>43445</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="3">
+      <c r="B12" s="8">
         <v>43446</v>
       </c>
       <c r="C12" t="s">
@@ -637,18 +655,18 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="3">
+      <c r="B13" s="8">
         <v>43447</v>
       </c>
       <c r="C13" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="3">
+      <c r="B14" s="8">
         <v>43448</v>
       </c>
       <c r="C14" t="s">
@@ -656,7 +674,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="3">
+      <c r="B15" s="8">
         <v>43449</v>
       </c>
       <c r="C15" t="s">
@@ -667,53 +685,53 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="8">
         <v>43451</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3">
+      <c r="B18" s="8">
         <v>43452</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3">
+      <c r="B19" s="8">
         <v>43453</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3">
+      <c r="B20" s="8">
         <v>43454</v>
       </c>
       <c r="C20" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
+      <c r="B21" s="8">
         <v>43455</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3">
+      <c r="B22" s="8">
         <v>43456</v>
       </c>
       <c r="C22" t="s">
@@ -724,7 +742,7 @@
       <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="8">
         <v>43458</v>
       </c>
       <c r="C24" t="s">
@@ -732,13 +750,16 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="3">
+      <c r="B25" s="8">
         <v>43459</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="3">
+      <c r="B26" s="8">
         <v>43460</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
u plan, nhanh hon x2 so voi du kien! very good ^^
</commit_message>
<xml_diff>
--- a/docs/plan.xlsx
+++ b/docs/plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>Thời gian</t>
   </si>
@@ -100,20 +100,10 @@
     <t>Hoàn thiện giao diện post, thêm database post</t>
   </si>
   <si>
-    <t>Làm giao diện trang detail post
-Làm API trả về ds post theo category</t>
-  </si>
-  <si>
-    <t>Hoàn thiện giao diện detail post,tìm hiểu cách đổ dữ liệu vào trang post</t>
-  </si>
-  <si>
     <t>Đổ dữ liệu vào trang post</t>
   </si>
   <si>
     <t>header("Location: page2.php?total=".$total);</t>
-  </si>
-  <si>
-    <t>Chuyển trang khi click, đổ dữ liệu vào detail post</t>
   </si>
   <si>
     <t>Tìm template</t>
@@ -139,6 +129,29 @@
   </si>
   <si>
     <t>Bắt sự kiện click 12 ngày, Lấy data-id nút bấm để gọi lên server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Làm API trả về ds post theo category</t>
+  </si>
+  <si>
+    <t>Làm giao diện trang detail post, Chuyển trang khi click
+Đổ dữ liệu vào detail post</t>
+  </si>
+  <si>
+    <t>Tìm hiểu cách đổ dữ liệu vào trang post</t>
+  </si>
+  <si>
+    <t>Việc mới</t>
+  </si>
+  <si>
+    <t>Làm giao diện trang cài đặt thông tin user</t>
+  </si>
+  <si>
+    <t>Chức năng đăng kí gửi email, đổi mật khẩu</t>
+  </si>
+  <si>
+    <t>Chức năng quên mật khẩu</t>
   </si>
 </sst>
 </file>
@@ -175,7 +188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -196,7 +209,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +233,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -227,6 +246,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -508,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -520,9 +543,10 @@
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="56.42578125" customWidth="1"/>
     <col min="4" max="4" width="45.42578125" customWidth="1"/>
+    <col min="5" max="5" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,138 +559,150 @@
       <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>43436</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>43437</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>43438</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>43439</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>43440</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="3">
         <v>43441</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="3">
         <v>43442</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="3">
         <v>43444</v>
       </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="C10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <v>43445</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <v>43446</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <v>43447</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
         <v>43448</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="3">
         <v>43449</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -677,8 +713,8 @@
       <c r="B17" s="3">
         <v>43451</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>24</v>
+      <c r="C17" s="8" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -686,7 +722,7 @@
         <v>43452</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,18 +730,18 @@
         <v>43453</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>43454</v>
       </c>
-      <c r="C20" t="s">
-        <v>28</v>
+      <c r="C20" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -713,10 +749,10 @@
         <v>43455</v>
       </c>
       <c r="C21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -735,7 +771,7 @@
         <v>43458</v>
       </c>
       <c r="C24" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>